<commit_message>
added CRUD-Matrix, renamed class diagram of software specification
</commit_message>
<xml_diff>
--- a/4_Entwurf/4_Anforderungen.xlsx
+++ b/4_Entwurf/4_Anforderungen.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Assistenz_Dienstplaner\GitHub_Repository\4_Entwurf\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alenn\Praxisprojekt_AssistenzDienstplaner\GitRepository\praxisprojekt_mi_bachelor_SoSe24\4_Entwurf\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E60684C-B712-486E-A31B-46C4281E48B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41ED629D-8105-4785-ACE9-9F3DC394E4B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{B727BAD2-A5BF-4C72-9515-F131A87DD358}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{B727BAD2-A5BF-4C72-9515-F131A87DD358}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -851,7 +851,59 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">Das System muss der dienstplanenden Person die Möglichkeit bieten, die Start- und Endzeiten sowie die Dauer der Schichten </t>
+      <t xml:space="preserve">Falls die dienstplanende Person Tags für Schichten und Assistent*innen angelegt hat, muss das System die Schichten und Assistent*innen gemäß der korrespondierenden Tags </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>zuordnen</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Sobald die Verfügbarkeiten aller Assistent*innen eingegeben oder importiert sind, muss das System einen optimalen Dienstplan unter Berücksichtigung der Voreinstellungen und deren Priorisierung/ Verbindlichkeiten </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>generieren</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Das System muss der dienstplanenden Person die Möglichkeit bieten, extern erfasste Abweichungen der geleisteten von den geplanten Arbeitsstunden der Assistent*innen </t>
     </r>
     <r>
       <rPr>
@@ -872,7 +924,85 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> und/ oder </t>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Das System muss der dienstplanenden Person die Möglichkeit bieten, ausbezahlte Überstunden aus der Stundendifferenz zu </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>entfernen</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Das System sollte fähig sein, die Urlaubsansprüche der Assistent*innen zu </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>berechnen</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> und </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>anzuzeigen</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Das System sollte der dienstplanenden Person die Möglichkeit bieten, die vertraglich vereinbarte Zahl an Urlaubstagen </t>
     </r>
     <r>
       <rPr>
@@ -898,59 +1028,7 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">Falls die dienstplanende Person Tags für Schichten und Assistent*innen angelegt hat, muss das System die Schichten und Assistent*innen gemäß der korrespondierenden Tags </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>zuordnen</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Sobald die Verfügbarkeiten aller Assistent*innen eingegeben oder importiert sind, muss das System einen optimalen Dienstplan unter Berücksichtigung der Voreinstellungen und deren Priorisierung/ Verbindlichkeiten </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>generieren</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Das System muss der dienstplanenden Person die Möglichkeit bieten, extern erfasste Abweichungen der geleisteten von den geplanten Arbeitsstunden der Assistent*innen </t>
+      <t xml:space="preserve">Das System sollte der dienstplanenden Person die Möglichkeit bieten, genehmigte Urlaubstage der Assistent*innen </t>
     </r>
     <r>
       <rPr>
@@ -976,106 +1054,203 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">Das System muss der dienstplanenden Person die Möglichkeit bieten, ausbezahlte Überstunden aus der Stundendifferenz zu </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>entfernen</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Das System sollte fähig sein, die Urlaubsansprüche der Assistent*innen zu </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>berechnen</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> und </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>anzuzeigen</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Das System sollte der dienstplanenden Person die Möglichkeit bieten, die vertraglich vereinbarte Zahl an Urlaubstagen </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>anzulegen</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Das System sollte der dienstplanenden Person die Möglichkeit bieten, genehmigte Urlaubstage der Assistent*innen </t>
+      <t xml:space="preserve">Sobald für eine Assistent*in genehmigte Urlaubstage eingegeben werden, muss das System die Urlaubsansprüche entsprechend </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>modifizieren</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <t>Verfügbarkeiten</t>
+  </si>
+  <si>
+    <t>Assistent*innen</t>
+  </si>
+  <si>
+    <t>Schichten</t>
+  </si>
+  <si>
+    <t>Tags</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Das System muss der dienstplanenden Person die Möglichkeit bieten, den angelegten Tags Prioritäten/ Verbindlichkeiten </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>zuzuordnen</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Sobald der Dienstplan generiert ist, muss das System der dienstplanenden Person die Möglichkeit bieten, die Zuordnung zwischen Assistent*innen und Schichten zu </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>bearbeiten</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">. </t>
+    </r>
+  </si>
+  <si>
+    <t>Hilfsfunktionen</t>
+  </si>
+  <si>
+    <t>Konflikte</t>
+  </si>
+  <si>
+    <t>Dienstplan</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Solange der Dienstplan gültig ist, muss das System der dienstplanenden Person die Möglichkeit bieten, Schichtzeiten und Zuordnungen zu </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>bearbeiten</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Das System sollte der dienstplanenden Person die Möglichkeit bieten, die Dienstplangenerierung beeinflussende Voreinstellungen </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>abzurufen</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, Prioritäten/ Verbindlichkeiten </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>zuzuordnen</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> und diese zu </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>bearbeiten</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Das System sollte der dienstplanenden Person die Möglichkeit bieten, zusätzliche Wünsche der Assistent*innen bezüglich der Einsatzzeiten </t>
     </r>
     <r>
       <rPr>
@@ -1096,23 +1271,107 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Sobald für eine Assistent*in genehmigte Urlaubstage eingegeben werden, muss das System die Urlaubsansprüche entsprechend </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>modifizieren</t>
+      <t xml:space="preserve"> und zu </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>speichern</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Das System muss der dienstplanenden Person die Möglichkeit bieten, Tags für Schichten mit besonderen Vorhaben </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">zu erstellen </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>und</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>den Schichten</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">und Assistent*innen </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>zuzuordnen</t>
     </r>
     <r>
       <rPr>
@@ -1138,192 +1397,22 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>anzulegen</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>.</t>
-    </r>
-  </si>
-  <si>
-    <t>Verfügbarkeiten</t>
-  </si>
-  <si>
-    <t>Assistent*innen</t>
-  </si>
-  <si>
-    <t>Schichten</t>
-  </si>
-  <si>
-    <t>Tags</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Das System muss der dienstplanenden Person die Möglichkeit bieten, den angelegten Tags Prioritäten/ Verbindlichkeiten </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>zuzuordnen</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Sobald der Dienstplan generiert ist, muss das System der dienstplanenden Person die Möglichkeit bieten, die Zuordnung zwischen Assistent*innen und Schichten zu </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>bearbeiten</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">. </t>
-    </r>
-  </si>
-  <si>
-    <t>Hilfsfunktionen</t>
-  </si>
-  <si>
-    <t>Konflikte</t>
-  </si>
-  <si>
-    <t>Dienstplan</t>
-  </si>
-  <si>
-    <t>x</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Solange der Dienstplan gültig ist, muss das System der dienstplanenden Person die Möglichkeit bieten, Schichtzeiten und Zuordnungen zu </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>bearbeiten</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Das System sollte der dienstplanenden Person die Möglichkeit bieten, die Dienstplangenerierung beeinflussende Voreinstellungen </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>abzurufen</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">, Prioritäten/ Verbindlichkeiten </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>zuzuordnen</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> und diese zu </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>bearbeiten</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Das System sollte der dienstplanenden Person die Möglichkeit bieten, zusätzliche Wünsche der Assistent*innen bezüglich der Einsatzzeiten </t>
+      <t>anzulegen und zu bearbeiten</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Das System muss der dienstplanenden Person die Möglichkeit bieten, die Start- und Endzeiten der Schichten </t>
     </r>
     <r>
       <rPr>
@@ -1344,107 +1433,18 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> und zu </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>speichern</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Das System muss der dienstplanenden Person die Möglichkeit bieten, Tags für Schichten mit besonderen Vorhaben </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">zu erstellen </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>und</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>den Schichten</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">und Assistent*innen </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>zuzuordnen</t>
+      <t xml:space="preserve"> oder </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>auszuwählen</t>
     </r>
     <r>
       <rPr>
@@ -1938,8 +1938,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{650723DC-46C9-46FE-B075-A3260489D6F9}">
   <dimension ref="A1:H41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1962,24 +1962,24 @@
         <v>1</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>25</v>
+        <v>48</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D2" s="5"/>
       <c r="E2" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="13"/>
       <c r="B3" s="5" t="s">
-        <v>34</v>
+        <v>47</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -1988,11 +1988,11 @@
         <v>3</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D4" s="8"/>
       <c r="E4" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
@@ -2001,11 +2001,11 @@
         <v>4</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D5" s="9"/>
       <c r="E5" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="58.8" customHeight="1" x14ac:dyDescent="0.3">
@@ -2015,33 +2015,33 @@
       </c>
       <c r="D6" s="10"/>
       <c r="E6" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="43.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="13"/>
       <c r="B7" s="9" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D7" s="11"/>
       <c r="E7" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="46.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="13"/>
       <c r="B8" s="9" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D8" s="12"/>
       <c r="E8" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="46.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -2050,16 +2050,16 @@
         <v>5</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A10" s="13"/>
       <c r="B10" s="10" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
@@ -2068,7 +2068,7 @@
         <v>11</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
@@ -2077,7 +2077,7 @@
         <v>6</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
@@ -2086,7 +2086,7 @@
         <v>7</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="43.8" customHeight="1" x14ac:dyDescent="0.3">
@@ -2101,16 +2101,16 @@
         <v>12</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A16" s="13"/>
       <c r="B16" s="8" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="71.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
@@ -2122,43 +2122,43 @@
     <row r="18" spans="1:3" ht="58.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="13"/>
       <c r="B18" s="10" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="46.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="13"/>
       <c r="B19" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="45.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="13"/>
       <c r="B20" s="10" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="45.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="13"/>
       <c r="B21" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="43.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="13"/>
       <c r="B22" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="13"/>
       <c r="B23" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="43.8" customHeight="1" x14ac:dyDescent="0.3">
@@ -2184,13 +2184,13 @@
     <row r="28" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A28" s="13"/>
       <c r="B28" s="10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A29" s="13"/>
       <c r="B29" s="9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
@@ -2256,13 +2256,13 @@
     <row r="40" spans="1:2" ht="31.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="13"/>
       <c r="B40" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A41" s="13"/>
       <c r="B41" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changes in CRUD matrix and requirements table
</commit_message>
<xml_diff>
--- a/4_Entwurf/4_Anforderungen.xlsx
+++ b/4_Entwurf/4_Anforderungen.xlsx
@@ -8,14 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alenn\Praxisprojekt_AssistenzDienstplaner\GitRepository\praxisprojekt_mi_bachelor_SoSe24\4_Entwurf\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41ED629D-8105-4785-ACE9-9F3DC394E4B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{E9EB3C2B-D836-4826-BCCB-E909FC57D77C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{B727BAD2-A5BF-4C72-9515-F131A87DD358}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
+    <sheet name="Tabelle2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -851,6 +853,53 @@
   </si>
   <si>
     <r>
+      <t xml:space="preserve">Das System muss der dienstplanenden Person die Möglichkeit bieten, die Start- und Endzeiten sowie die Dauer der Schichten </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>einzugeben</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> und/ oder </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>anzulegen</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <r>
       <t xml:space="preserve">Falls die dienstplanende Person Tags für Schichten und Assistent*innen angelegt hat, muss das System die Schichten und Assistent*innen gemäß der korrespondierenden Tags </t>
     </r>
     <r>
@@ -1079,6 +1128,32 @@
     </r>
   </si>
   <si>
+    <r>
+      <t xml:space="preserve">Das System muss der dienstplanenden Person die Möglichkeit bieten, Assistent*innen </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>anzulegen</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
     <t>Verfügbarkeiten</t>
   </si>
   <si>
@@ -1372,79 +1447,6 @@
         <scheme val="minor"/>
       </rPr>
       <t>zuzuordnen</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Das System muss der dienstplanenden Person die Möglichkeit bieten, Assistent*innen </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>anzulegen und zu bearbeiten</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Das System muss der dienstplanenden Person die Möglichkeit bieten, die Start- und Endzeiten der Schichten </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>einzugeben</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> oder </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>auszuwählen</t>
     </r>
     <r>
       <rPr>
@@ -1938,8 +1940,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{650723DC-46C9-46FE-B075-A3260489D6F9}">
   <dimension ref="A1:H41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1962,24 +1964,24 @@
         <v>1</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>48</v>
+        <v>25</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="D2" s="5"/>
       <c r="E2" s="2" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="13"/>
       <c r="B3" s="5" t="s">
-        <v>47</v>
+        <v>34</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="2" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -1988,11 +1990,11 @@
         <v>3</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="D4" s="8"/>
       <c r="E4" s="2" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
@@ -2001,11 +2003,11 @@
         <v>4</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="D5" s="9"/>
       <c r="E5" s="2" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="58.8" customHeight="1" x14ac:dyDescent="0.3">
@@ -2015,33 +2017,33 @@
       </c>
       <c r="D6" s="10"/>
       <c r="E6" s="2" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="43.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="13"/>
       <c r="B7" s="9" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="D7" s="11"/>
       <c r="E7" s="2" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="46.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="13"/>
       <c r="B8" s="9" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="D8" s="12"/>
       <c r="E8" s="2" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="46.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -2050,16 +2052,16 @@
         <v>5</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A10" s="13"/>
       <c r="B10" s="10" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
@@ -2068,7 +2070,7 @@
         <v>11</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
@@ -2077,7 +2079,7 @@
         <v>6</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
@@ -2086,7 +2088,7 @@
         <v>7</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="43.8" customHeight="1" x14ac:dyDescent="0.3">
@@ -2101,16 +2103,16 @@
         <v>12</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A16" s="13"/>
       <c r="B16" s="8" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="71.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
@@ -2122,43 +2124,43 @@
     <row r="18" spans="1:3" ht="58.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="13"/>
       <c r="B18" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="C18" s="2" t="s">
         <v>44</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="46.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="13"/>
       <c r="B19" s="5" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="45.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="13"/>
       <c r="B20" s="10" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="45.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="13"/>
       <c r="B21" s="5" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="43.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="13"/>
       <c r="B22" s="5" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="13"/>
       <c r="B23" s="5" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="43.8" customHeight="1" x14ac:dyDescent="0.3">
@@ -2184,13 +2186,13 @@
     <row r="28" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A28" s="13"/>
       <c r="B28" s="10" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A29" s="13"/>
       <c r="B29" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
@@ -2256,13 +2258,13 @@
     <row r="40" spans="1:2" ht="31.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="13"/>
       <c r="B40" s="5" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A41" s="13"/>
       <c r="B41" s="5" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -2272,4 +2274,16 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D838353A-6E16-4B91-A1A3-F609BDEB3AD0}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>